<commit_message>
Realign ids names and titles for all new profiles for consistency [FHIR-36728](https://jira.hl7.org/browse/FHIR-36728)
</commit_message>
<xml_diff>
--- a/input/images/uscdi_table.xlsx
+++ b/input/images/uscdi_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F35C532-7F7E-3A48-BF1B-44E9EDA6B1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BA4FE2-5AD1-B44E-B6E4-40359163B79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="47020" windowHeight="27580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="165">
   <si>
     <t>USCDI v2 Summary of Data Classes and Data Elements</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Clinical Test</t>
   </si>
   <si>
-    <t>US Core Clinical Test Result Observation Profile, US Core DiagnosticReport Profile for Report and Note exchange</t>
-  </si>
-  <si>
     <t>Observation, DiagnosticReport</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>Diagnostic Imaging Test</t>
   </si>
   <si>
-    <t>US Core Diagnostic Imaging Result Observation Profile, US Core DiagnosticReport Profile for Report and Note exchange</t>
-  </si>
-  <si>
     <t>Diagnostic Imaging Result/Report</t>
   </si>
   <si>
@@ -190,9 +184,6 @@
     <t>Diagnosis</t>
   </si>
   <si>
-    <t>US Core Condition Profile</t>
-  </si>
-  <si>
     <t>Condition.code</t>
   </si>
   <si>
@@ -391,9 +382,6 @@
     <t>Sexual Orientation</t>
   </si>
   <si>
-    <t>US Core Sexual Orientation Observation Profile</t>
-  </si>
-  <si>
     <t>Observation</t>
   </si>
   <si>
@@ -403,9 +391,6 @@
     <t>Assessment</t>
   </si>
   <si>
-    <t>US Core Screening Response Observation Profile,US Core Social History Assessment Observation Profile</t>
-  </si>
-  <si>
     <t>Goals</t>
   </si>
   <si>
@@ -505,13 +490,31 @@
     <t>US Core Pediatric Head Occipital Frontal Circumference Observation Profile (Builds on Us Core Vital Signs Profile)</t>
   </si>
   <si>
-    <t>US Core Diagnostic Imaging Test Result Observation Profile, US Core DiagnosticReport Profile for Report and Note exchange</t>
-  </si>
-  <si>
     <t>US Core Medication Profile,  US Core Medication Request Profile</t>
   </si>
   <si>
     <t>Medication, MedicationRequest</t>
+  </si>
+  <si>
+    <t>US Core Condition Problems and Health Concerns Profile</t>
+  </si>
+  <si>
+    <t>US Core Condition Encounter Diagnosis Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Diagnostic Imaging Result Profile, US Core DiagnosticReport Profile for Report and Note exchange</t>
+  </si>
+  <si>
+    <t>US Core Observation Clinical Test Result Profile, US Core DiagnosticReport Profile for Report and Note exchange</t>
+  </si>
+  <si>
+    <t>US Core Observation Sexual Orientation Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation SDOH Assessment Profile,US Core Observation Social History Profile, US Core QuestionnaireResponse Profile</t>
+  </si>
+  <si>
+    <t>Observation, QuestionnaireResponse</t>
   </si>
 </sst>
 </file>
@@ -890,7 +893,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1212,10 +1217,10 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
+        <v>161</v>
+      </c>
+      <c r="C23" t="s">
         <v>44</v>
-      </c>
-      <c r="C23" t="s">
-        <v>45</v>
       </c>
       <c r="D23" t="s">
         <v>3</v>
@@ -1223,13 +1228,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" t="s">
         <v>44</v>
-      </c>
-      <c r="C24" t="s">
-        <v>45</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
@@ -1237,7 +1242,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
@@ -1251,13 +1256,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>160</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" t="s">
         <v>3</v>
@@ -1265,13 +1270,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
         <v>3</v>
@@ -1279,10 +1284,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -1293,13 +1298,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
         <v>52</v>
-      </c>
-      <c r="C29" t="s">
-        <v>54</v>
       </c>
       <c r="D29" t="s">
         <v>3</v>
@@ -1307,13 +1312,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>159</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
         <v>3</v>
@@ -1321,13 +1326,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
         <v>3</v>
@@ -1338,10 +1343,10 @@
         <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D32" t="s">
         <v>3</v>
@@ -1349,13 +1354,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
         <v>3</v>
@@ -1363,7 +1368,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
@@ -1377,13 +1382,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
         <v>3</v>
@@ -1391,13 +1396,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D36" t="s">
         <v>3</v>
@@ -1405,13 +1410,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D37" t="s">
         <v>3</v>
@@ -1419,7 +1424,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
@@ -1433,13 +1438,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D39" t="s">
         <v>3</v>
@@ -1447,13 +1452,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D40" t="s">
         <v>3</v>
@@ -1461,7 +1466,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
@@ -1475,13 +1480,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D42" t="s">
         <v>3</v>
@@ -1489,7 +1494,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
         <v>6</v>
@@ -1503,7 +1508,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
@@ -1517,13 +1522,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s">
         <v>3</v>
@@ -1531,13 +1536,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" t="s">
         <v>81</v>
-      </c>
-      <c r="C46" t="s">
-        <v>84</v>
       </c>
       <c r="D46" t="s">
         <v>3</v>
@@ -1545,13 +1550,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D47" t="s">
         <v>3</v>
@@ -1559,13 +1564,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D48" t="s">
         <v>3</v>
@@ -1573,13 +1578,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D49" t="s">
         <v>3</v>
@@ -1587,13 +1592,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D50" t="s">
         <v>3</v>
@@ -1601,13 +1606,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D51" t="s">
         <v>3</v>
@@ -1615,13 +1620,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D52" t="s">
         <v>3</v>
@@ -1629,13 +1634,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C53" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D53" t="s">
         <v>3</v>
@@ -1643,13 +1648,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C54" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D54" t="s">
         <v>3</v>
@@ -1657,13 +1662,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C55" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D55" t="s">
         <v>3</v>
@@ -1671,13 +1676,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C56" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D56" t="s">
         <v>3</v>
@@ -1685,13 +1690,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C57" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D57" t="s">
         <v>3</v>
@@ -1699,13 +1704,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B58" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D58" t="s">
         <v>3</v>
@@ -1713,13 +1718,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D59" t="s">
         <v>3</v>
@@ -1727,13 +1732,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="C60" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D60" t="s">
         <v>3</v>
@@ -1741,13 +1746,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="C61" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D61" t="s">
         <v>3</v>
@@ -1755,13 +1760,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="C62" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D62" t="s">
         <v>3</v>
@@ -1769,10 +1774,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B63" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
@@ -1783,13 +1788,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C64" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D64" t="s">
         <v>3</v>
@@ -1797,13 +1802,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B65" t="s">
+        <v>113</v>
+      </c>
+      <c r="C65" t="s">
         <v>116</v>
-      </c>
-      <c r="C65" t="s">
-        <v>119</v>
       </c>
       <c r="D65" t="s">
         <v>3</v>
@@ -1811,13 +1816,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B66" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C66" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D66" t="s">
         <v>3</v>
@@ -1825,13 +1830,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B67" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="C67" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D67" t="s">
         <v>3</v>
@@ -1839,7 +1844,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B68" t="s">
         <v>3</v>
@@ -1853,13 +1858,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B69" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="C69" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="D69" t="s">
         <v>3</v>
@@ -1867,13 +1872,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B70" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C70" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D70" t="s">
         <v>3</v>
@@ -1881,13 +1886,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B71" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C71" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D71" t="s">
         <v>3</v>
@@ -1895,13 +1900,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B72" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="C72" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D72" t="s">
         <v>3</v>
@@ -1909,13 +1914,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B73" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C73" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D73" t="s">
         <v>3</v>
@@ -1923,13 +1928,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B74" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C74" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D74" t="s">
         <v>3</v>
@@ -1937,7 +1942,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B75" t="s">
         <v>3</v>
@@ -1951,13 +1956,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B76" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C76" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D76" t="s">
         <v>3</v>
@@ -1965,13 +1970,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B77" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C77" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D77" t="s">
         <v>3</v>
@@ -1979,13 +1984,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B78" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C78" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D78" t="s">
         <v>3</v>
@@ -1993,13 +1998,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C79" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D79" t="s">
         <v>3</v>
@@ -2007,13 +2012,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C80" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D80" t="s">
         <v>3</v>
@@ -2021,13 +2026,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B81" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C81" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D81" t="s">
         <v>3</v>
@@ -2035,13 +2040,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B82" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C82" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D82" t="s">
         <v>3</v>
@@ -2049,13 +2054,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B83" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C83" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D83" t="s">
         <v>3</v>
@@ -2063,13 +2068,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B84" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C84" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D84" t="s">
         <v>3</v>
@@ -2077,13 +2082,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B85" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C85" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D85" t="s">
         <v>3</v>
@@ -2091,13 +2096,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B86" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C86" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D86" t="s">
         <v>3</v>
@@ -2105,13 +2110,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B87" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C87" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D87" t="s">
         <v>3</v>
@@ -2120,7 +2125,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E26 A33:E41 A32:B32 D32:E32 A28:E31 A27 C27:E27 A43:E89 A42 D42:E42" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E22 A33:E35 A32:B32 D32:E32 A28:E29 A27 C27:E27 A43:E59 A42 D42:E42 A37:E41 A36 C36:E36 A31:E31 A30 C30:E30 A63:E66 A60 C60:E60 A61 C61:E61 A62 C62:E62 A73:E89 A72 C72:E72 A26 C26:E26 A25:E25 A23 C23:E23 A24 C24:E24 A68:E68 A67 C67:E67 A70:E71 A69 D69:E69" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
QA fix USCDI table
</commit_message>
<xml_diff>
--- a/input/images/uscdi_table.xlsx
+++ b/input/images/uscdi_table.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5ED8CC4A-56FD-E043-ABED-4D687A0B24FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CB32CE72-B132-EA47-9E21-4BAECD1D9D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="500" windowWidth="34120" windowHeight="28300"/>
+    <workbookView xWindow="30280" yWindow="500" windowWidth="51200" windowHeight="28300"/>
   </bookViews>
   <sheets>
     <sheet name="uscdi_table" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="472" uniqueCount="233">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="467" uniqueCount="226">
   <si>
     <t>data_class</t>
   </si>
@@ -78,15 +89,6 @@
     <t>SDOH Assessment</t>
   </si>
   <si>
-    <t>US Core Observation SDOH Assessment Profile|US Core Observation Social History Profile| US Core QuestionnaireResponse Profile</t>
-  </si>
-  <si>
-    <t>Observation, QuestionnaireResponse</t>
-  </si>
-  <si>
-    <t>See SDOH Guidance</t>
-  </si>
-  <si>
     <t>Care Team Members</t>
   </si>
   <si>
@@ -183,7 +185,7 @@
     <t>Clinical Tests</t>
   </si>
   <si>
-    <t>US Core Observation Clinical Test Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
+    <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
   </si>
   <si>
     <t>Clinical Test</t>
@@ -198,9 +200,6 @@
     <t>Diagnostic Imaging</t>
   </si>
   <si>
-    <t>US Core Observation Imaging Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
-  </si>
-  <si>
     <t>Diagnostic Imaging Test</t>
   </si>
   <si>
@@ -237,15 +236,6 @@
     <t>Encounter.period</t>
   </si>
   <si>
-    <t>Foo</t>
-  </si>
-  <si>
-    <t>US Core Foo Profile</t>
-  </si>
-  <si>
-    <t>Bar</t>
-  </si>
-  <si>
     <t>Encounter.location.location</t>
   </si>
   <si>
@@ -543,7 +533,7 @@
     <t>Phone Number</t>
   </si>
   <si>
-    <t>Related Person’s Name</t>
+    <t>Related Person's Name</t>
   </si>
   <si>
     <t>US Core RelatedPerson Profile</t>
@@ -552,7 +542,7 @@
     <t>RelatedPerson.name</t>
   </si>
   <si>
-    <t>Related Person’s Relationship</t>
+    <t>Related Person's Relationship</t>
   </si>
   <si>
     <t>RelatedPerson.relationship</t>
@@ -564,15 +554,9 @@
     <t>US Core Observation Occupation Profile</t>
   </si>
   <si>
-    <t>Observation/QR ????</t>
-  </si>
-  <si>
     <t>Occupation Industry</t>
   </si>
   <si>
-    <t>Observation/QR ???</t>
-  </si>
-  <si>
     <t>Problems</t>
   </si>
   <si>
@@ -648,7 +632,7 @@
     <t>Device</t>
   </si>
   <si>
-    <t>Unique Device Identifier(s) for a Patient’s Implantable Device(s)</t>
+    <t>Unique Device Identifier(s) for a Patient's Implantable Device(s)</t>
   </si>
   <si>
     <t>Vital Signs</t>
@@ -717,13 +701,19 @@
     <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
   </si>
   <si>
-    <t>Occipital-frontal Head Circumference Percentile (Birth - 36 months)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US Core Pediatric Head Occipital Frontal Circumference Observation Profile </t>
-  </si>
-  <si>
-    <t>US Core Observation Screening and Assessments Profile</t>
+    <t>Occipital Frontal Head Circumference Percentile (Birth - 36 months)</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>US Core Sex For Clinical Use Extension</t>
+  </si>
+  <si>
+    <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
   </si>
 </sst>
 </file>
@@ -1207,8 +1197,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1564,18 +1555,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="111.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="50.33203125" customWidth="1"/>
+    <col min="3" max="3" width="111.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="50.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1666,1566 +1656,1549 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
+        <v>225</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
         <v>30</v>
-      </c>
-      <c r="E13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>39</v>
-      </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>39</v>
-      </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s">
-        <v>39</v>
-      </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" t="s">
         <v>36</v>
       </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" t="s">
-        <v>39</v>
-      </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" t="s">
         <v>51</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" t="s">
         <v>51</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
         <v>56</v>
       </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E31" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" t="s">
         <v>61</v>
       </c>
-      <c r="B32" t="s">
-        <v>65</v>
-      </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E33" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" t="s">
-        <v>71</v>
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" t="s">
-        <v>71</v>
-      </c>
-      <c r="F35" t="s">
-        <v>72</v>
+        <v>67</v>
+      </c>
+      <c r="D35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" t="s">
-        <v>62</v>
-      </c>
-      <c r="E36" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E37" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F38" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" t="s">
         <v>76</v>
       </c>
-      <c r="B40" t="s">
-        <v>80</v>
+      <c r="D40" t="s">
+        <v>75</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
-      </c>
-      <c r="F40" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" t="s">
-        <v>82</v>
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" t="s">
         <v>81</v>
-      </c>
-      <c r="B42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" t="s">
-        <v>82</v>
-      </c>
-      <c r="E42" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D44" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E44" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D45" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E45" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D46" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E46" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
-      </c>
-      <c r="D47" t="s">
-        <v>82</v>
-      </c>
-      <c r="E47" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>91</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
       </c>
       <c r="D48" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="E48" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+      <c r="C49" t="s">
+        <v>225</v>
+      </c>
+      <c r="D49" t="s">
+        <v>225</v>
+      </c>
+      <c r="E49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F49" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" t="s">
         <v>97</v>
       </c>
-      <c r="B50" t="s">
-        <v>98</v>
-      </c>
-      <c r="C50" t="s">
-        <v>99</v>
-      </c>
       <c r="D50" t="s">
-        <v>99</v>
+        <v>225</v>
       </c>
       <c r="E50" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
-      </c>
-      <c r="C51" t="s">
-        <v>232</v>
+        <v>98</v>
       </c>
       <c r="D51" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E51" t="s">
-        <v>102</v>
-      </c>
-      <c r="F51" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C52" t="s">
-        <v>232</v>
+        <v>100</v>
       </c>
       <c r="D52" t="s">
-        <v>232</v>
+        <v>100</v>
       </c>
       <c r="E52" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>232</v>
+        <v>102</v>
       </c>
       <c r="D53" t="s">
-        <v>232</v>
+        <v>102</v>
       </c>
       <c r="E53" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>97</v>
-      </c>
-      <c r="B54" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D54" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E54" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>97</v>
-      </c>
-      <c r="B55" t="s">
-        <v>108</v>
-      </c>
-      <c r="C55" t="s">
-        <v>109</v>
-      </c>
-      <c r="D55" t="s">
-        <v>109</v>
-      </c>
-      <c r="E55" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
-      </c>
-      <c r="D56" t="s">
-        <v>111</v>
-      </c>
-      <c r="E56" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>110</v>
+        <v>106</v>
+      </c>
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="D57" t="s">
+        <v>107</v>
+      </c>
+      <c r="E57" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>113</v>
-      </c>
-      <c r="C58" t="s">
-        <v>114</v>
+        <v>106</v>
+      </c>
+      <c r="B58" t="s">
+        <v>109</v>
+      </c>
+      <c r="D58" t="s">
+        <v>107</v>
+      </c>
+      <c r="E58" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D59" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E59" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" t="s">
         <v>113</v>
       </c>
-      <c r="B60" t="s">
-        <v>116</v>
-      </c>
       <c r="D60" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E60" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" t="s">
-        <v>117</v>
-      </c>
-      <c r="D61" t="s">
-        <v>118</v>
-      </c>
-      <c r="E61" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+      <c r="C61" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D62" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E62" t="s">
-        <v>54</v>
+        <v>117</v>
+      </c>
+      <c r="F62" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" t="s">
+        <v>119</v>
+      </c>
+      <c r="D63" t="s">
+        <v>120</v>
+      </c>
+      <c r="E63" t="s">
         <v>121</v>
-      </c>
-      <c r="C63" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>114</v>
+      </c>
+      <c r="B64" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64" t="s">
+        <v>120</v>
+      </c>
+      <c r="E64" t="s">
         <v>121</v>
-      </c>
-      <c r="B64" t="s">
-        <v>121</v>
-      </c>
-      <c r="D64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E64" t="s">
-        <v>124</v>
-      </c>
-      <c r="F64" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" t="s">
+        <v>120</v>
+      </c>
+      <c r="E65" t="s">
         <v>121</v>
-      </c>
-      <c r="B65" t="s">
-        <v>126</v>
-      </c>
-      <c r="D65" t="s">
-        <v>127</v>
-      </c>
-      <c r="E65" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>124</v>
+      </c>
+      <c r="C66" t="s">
+        <v>125</v>
       </c>
       <c r="D66" t="s">
+        <v>126</v>
+      </c>
+      <c r="E66" t="s">
         <v>127</v>
-      </c>
-      <c r="E66" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>121</v>
-      </c>
-      <c r="B67" t="s">
-        <v>130</v>
-      </c>
-      <c r="D67" t="s">
-        <v>127</v>
-      </c>
-      <c r="E67" t="s">
         <v>128</v>
+      </c>
+      <c r="C67" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B68" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" t="s">
+        <v>129</v>
+      </c>
+      <c r="E68" t="s">
         <v>131</v>
-      </c>
-      <c r="C68" t="s">
-        <v>132</v>
-      </c>
-      <c r="D68" t="s">
-        <v>133</v>
-      </c>
-      <c r="E68" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>135</v>
-      </c>
-      <c r="C69" t="s">
-        <v>136</v>
+        <v>128</v>
+      </c>
+      <c r="B69" t="s">
+        <v>132</v>
+      </c>
+      <c r="D69" t="s">
+        <v>129</v>
+      </c>
+      <c r="E69" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>128</v>
+      </c>
+      <c r="B70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D70" t="s">
+        <v>129</v>
+      </c>
+      <c r="E70" t="s">
         <v>135</v>
-      </c>
-      <c r="B70" t="s">
-        <v>137</v>
-      </c>
-      <c r="D70" t="s">
-        <v>136</v>
-      </c>
-      <c r="E70" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B71" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D71" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E71" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B72" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D72" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E72" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D73" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E73" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B74" t="s">
-        <v>144</v>
+        <v>222</v>
       </c>
       <c r="D74" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E74" t="s">
-        <v>145</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B75" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D75" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E75" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B76" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D76" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E76" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B77" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="C77" t="s">
+        <v>146</v>
       </c>
       <c r="D77" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E77" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C78" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D78" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E78" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C79" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D79" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E79" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B80" t="s">
+        <v>152</v>
+      </c>
+      <c r="C80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D80" t="s">
+        <v>129</v>
+      </c>
+      <c r="E80" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>128</v>
+      </c>
+      <c r="B81" t="s">
+        <v>155</v>
+      </c>
+      <c r="C81" t="s">
         <v>156</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D81" t="s">
+        <v>156</v>
+      </c>
+      <c r="E81" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>128</v>
+      </c>
+      <c r="B82" t="s">
         <v>157</v>
       </c>
-      <c r="D80" t="s">
-        <v>136</v>
-      </c>
-      <c r="E80" t="s">
+      <c r="D82" t="s">
+        <v>129</v>
+      </c>
+      <c r="E82" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>135</v>
-      </c>
-      <c r="B81" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>128</v>
+      </c>
+      <c r="B83" t="s">
         <v>159</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D83" t="s">
+        <v>129</v>
+      </c>
+      <c r="E83" t="s">
         <v>160</v>
       </c>
-      <c r="D81" t="s">
-        <v>136</v>
-      </c>
-      <c r="E81" t="s">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>128</v>
+      </c>
+      <c r="B84" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>135</v>
-      </c>
-      <c r="B82" t="s">
+      <c r="D84" t="s">
+        <v>129</v>
+      </c>
+      <c r="E84" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>128</v>
+      </c>
+      <c r="B85" t="s">
         <v>162</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D85" t="s">
+        <v>129</v>
+      </c>
+      <c r="E85" t="s">
         <v>163</v>
       </c>
-      <c r="D82" t="s">
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>128</v>
+      </c>
+      <c r="B86" t="s">
+        <v>164</v>
+      </c>
+      <c r="D86" t="s">
+        <v>129</v>
+      </c>
+      <c r="E86" t="s">
         <v>163</v>
       </c>
-      <c r="E82" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>135</v>
-      </c>
-      <c r="B83" t="s">
-        <v>164</v>
-      </c>
-      <c r="D83" t="s">
-        <v>136</v>
-      </c>
-      <c r="E83" t="s">
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>135</v>
-      </c>
-      <c r="B84" t="s">
+      <c r="C87" t="s">
         <v>166</v>
       </c>
-      <c r="D84" t="s">
-        <v>136</v>
-      </c>
-      <c r="E84" t="s">
+      <c r="D87" t="s">
+        <v>166</v>
+      </c>
+      <c r="E87" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>135</v>
-      </c>
-      <c r="B85" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>128</v>
+      </c>
+      <c r="B88" t="s">
         <v>168</v>
       </c>
-      <c r="D85" t="s">
-        <v>136</v>
-      </c>
-      <c r="E85" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>135</v>
-      </c>
-      <c r="B86" t="s">
+      <c r="C88" t="s">
+        <v>166</v>
+      </c>
+      <c r="D88" t="s">
+        <v>166</v>
+      </c>
+      <c r="E88" t="s">
         <v>169</v>
       </c>
-      <c r="D86" t="s">
-        <v>136</v>
-      </c>
-      <c r="E86" t="s">
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>128</v>
+      </c>
+      <c r="B89" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>135</v>
-      </c>
-      <c r="B87" t="s">
+      <c r="C89" t="s">
         <v>171</v>
       </c>
-      <c r="D87" t="s">
-        <v>136</v>
-      </c>
-      <c r="E87" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>135</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="D89" t="s">
+        <v>171</v>
+      </c>
+      <c r="E89" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>128</v>
+      </c>
+      <c r="B90" t="s">
         <v>172</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C90" t="s">
+        <v>171</v>
+      </c>
+      <c r="D90" t="s">
+        <v>171</v>
+      </c>
+      <c r="E90" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>173</v>
       </c>
-      <c r="D88" t="s">
+      <c r="C91" t="s">
+        <v>92</v>
+      </c>
+      <c r="D91" t="s">
+        <v>92</v>
+      </c>
+      <c r="E91" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>173</v>
       </c>
-      <c r="E88" t="s">
+      <c r="B92" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>135</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="D92" t="s">
+        <v>92</v>
+      </c>
+      <c r="E92" t="s">
         <v>175</v>
       </c>
-      <c r="C89" t="s">
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>173</v>
       </c>
-      <c r="D89" t="s">
+      <c r="B93" t="s">
+        <v>176</v>
+      </c>
+      <c r="D93" t="s">
+        <v>92</v>
+      </c>
+      <c r="E93" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>173</v>
       </c>
-      <c r="E89" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>135</v>
-      </c>
-      <c r="B90" t="s">
-        <v>177</v>
-      </c>
-      <c r="C90" t="s">
+      <c r="B94" t="s">
         <v>178</v>
       </c>
-      <c r="D90" t="s">
-        <v>178</v>
-      </c>
-      <c r="E90" t="s">
+      <c r="D94" t="s">
+        <v>92</v>
+      </c>
+      <c r="E94" t="s">
+        <v>93</v>
+      </c>
+      <c r="F94" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>135</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="C95" t="s">
         <v>180</v>
       </c>
-      <c r="C91" t="s">
-        <v>178</v>
-      </c>
-      <c r="D91" t="s">
-        <v>178</v>
-      </c>
-      <c r="E91" t="s">
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>179</v>
+      </c>
+      <c r="B96" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>182</v>
-      </c>
-      <c r="C92" t="s">
-        <v>99</v>
-      </c>
-      <c r="D92" t="s">
-        <v>99</v>
-      </c>
-      <c r="E92" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>182</v>
-      </c>
-      <c r="B93" t="s">
-        <v>183</v>
-      </c>
-      <c r="D93" t="s">
-        <v>99</v>
-      </c>
-      <c r="E93" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>182</v>
-      </c>
-      <c r="B94" t="s">
-        <v>185</v>
-      </c>
-      <c r="D94" t="s">
-        <v>99</v>
-      </c>
-      <c r="E94" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>182</v>
-      </c>
-      <c r="B95" t="s">
-        <v>187</v>
-      </c>
-      <c r="D95" t="s">
-        <v>99</v>
-      </c>
-      <c r="E95" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>188</v>
-      </c>
-      <c r="C96" t="s">
-        <v>189</v>
+      <c r="D96" t="s">
+        <v>180</v>
+      </c>
+      <c r="E96" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B97" t="s">
-        <v>190</v>
+        <v>182</v>
+      </c>
+      <c r="C97" t="s">
+        <v>183</v>
       </c>
       <c r="D97" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E97" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B98" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C98" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D98" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E98" t="s">
-        <v>193</v>
+        <v>187</v>
+      </c>
+      <c r="F98" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>188</v>
       </c>
-      <c r="B99" t="s">
-        <v>194</v>
-      </c>
       <c r="C99" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D99" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E99" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F99" t="s">
-        <v>19</v>
+        <v>190</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>197</v>
-      </c>
-      <c r="C100" t="s">
-        <v>198</v>
+        <v>188</v>
+      </c>
+      <c r="B100" t="s">
+        <v>191</v>
       </c>
       <c r="D100" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E100" t="s">
-        <v>197</v>
-      </c>
-      <c r="F100" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D101" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E101" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>195</v>
+      </c>
+      <c r="C102" t="s">
+        <v>196</v>
+      </c>
+      <c r="D102" t="s">
+        <v>196</v>
+      </c>
+      <c r="E102" t="s">
         <v>197</v>
-      </c>
-      <c r="B102" t="s">
-        <v>202</v>
-      </c>
-      <c r="D102" t="s">
-        <v>198</v>
-      </c>
-      <c r="E102" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>204</v>
-      </c>
-      <c r="C103" t="s">
-        <v>205</v>
+        <v>195</v>
+      </c>
+      <c r="B103" t="s">
+        <v>198</v>
       </c>
       <c r="D103" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E103" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>204</v>
-      </c>
-      <c r="B104" t="s">
-        <v>207</v>
-      </c>
-      <c r="D104" t="s">
-        <v>205</v>
-      </c>
-      <c r="E104" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="C104" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>199</v>
+      </c>
+      <c r="B105" t="s">
+        <v>201</v>
       </c>
       <c r="C105" t="s">
-        <v>209</v>
+        <v>202</v>
+      </c>
+      <c r="D105" t="s">
+        <v>202</v>
+      </c>
+      <c r="E105" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B106" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C106" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D106" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="E106" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C107" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D107" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E107" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B108" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C108" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D108" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E108" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>199</v>
+      </c>
+      <c r="B109" t="s">
         <v>208</v>
       </c>
-      <c r="B109" t="s">
-        <v>215</v>
-      </c>
       <c r="C109" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D109" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E109" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B110" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C110" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D110" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="E110" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B111" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C111" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D111" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E111" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B112" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C112" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D112" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E112" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B113" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C113" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D113" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E113" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B114" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C114" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D114" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E114" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B115" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C115" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D115" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E115" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B116" t="s">
-        <v>228</v>
-      </c>
-      <c r="C116" t="s">
-        <v>229</v>
-      </c>
-      <c r="D116" t="s">
-        <v>229</v>
+        <v>221</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E116" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>208</v>
-      </c>
-      <c r="B117" t="s">
-        <v>230</v>
-      </c>
-      <c r="C117" t="s">
-        <v>231</v>
-      </c>
-      <c r="D117" t="s">
-        <v>231</v>
-      </c>
-      <c r="E117" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QA updates to change log
</commit_message>
<xml_diff>
--- a/input/images/uscdi_table.xlsx
+++ b/input/images/uscdi_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CB32CE72-B132-EA47-9E21-4BAECD1D9D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0D94F06D-3DC0-1440-B196-F3D30D8E771C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30280" yWindow="500" windowWidth="51200" windowHeight="28300"/>
   </bookViews>
@@ -1558,7 +1558,7 @@
   <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
qa fix errors in uscdi_table.csv and uscdi_table.xlsx
</commit_message>
<xml_diff>
--- a/input/images/uscdi_table.xlsx
+++ b/input/images/uscdi_table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B675C468-9B94-BC4A-B11B-D70BC7A0EAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{85DF82AE-FE25-0742-993D-0F226D92A9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="500" windowWidth="51200" windowHeight="28300"/>
+    <workbookView xWindow="-48100" yWindow="-18220" windowWidth="43220" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="uscdi_table" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="551" uniqueCount="245">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="551" uniqueCount="246">
   <si>
     <t>data_class</t>
   </si>
@@ -428,9 +428,6 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>US Core Sex For Clinical Use Extension</t>
-  </si>
-  <si>
     <t>Date of Birth</t>
   </si>
   <si>
@@ -458,18 +455,12 @@
     <t>Tribal Affiliation</t>
   </si>
   <si>
-    <t>US Core Tribal Affiliation Extension</t>
-  </si>
-  <si>
     <t>US Core Tibal Affiliation Extension</t>
   </si>
   <si>
     <t>Gender Identity</t>
   </si>
   <si>
-    <t>US Core Gender Identity Extension</t>
-  </si>
-  <si>
     <t>Gender Identity Extension</t>
   </si>
   <si>
@@ -771,12 +762,24 @@
   </si>
   <si>
     <t>See Screening and Assessments Guidance</t>
+  </si>
+  <si>
+    <t>US Core Patient Profile | US Core Birth Sex Extension</t>
+  </si>
+  <si>
+    <t>US Core Patient Profile | US Core Ethnicity Extension</t>
+  </si>
+  <si>
+    <t>US Core Patient Profile | US Core Tribal Affiliation Extension</t>
+  </si>
+  <si>
+    <t>US Core Patient Profile | US Core Gender Identity Extension</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1619,11 +1622,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F108" sqref="F108"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1648,7 +1651,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1682,7 +1685,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1696,7 +1699,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1710,7 +1713,7 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1718,13 +1721,13 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1746,16 +1749,16 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1789,7 +1792,7 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1806,7 +1809,7 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1823,7 +1826,7 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1840,7 +1843,7 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2256,7 +2259,7 @@
         <v>68</v>
       </c>
       <c r="G38" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -2270,7 +2273,7 @@
         <v>71</v>
       </c>
       <c r="F39" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2400,13 +2403,13 @@
         <v>86</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D47" t="s">
         <v>86</v>
       </c>
       <c r="F47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2431,7 +2434,7 @@
         <v>86</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D49" t="s">
         <v>90</v>
@@ -2443,7 +2446,7 @@
         <v>16</v>
       </c>
       <c r="G49" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -2451,7 +2454,7 @@
         <v>86</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D50" t="s">
         <v>91</v>
@@ -2468,7 +2471,7 @@
         <v>86</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D51" t="s">
         <v>92</v>
@@ -2550,10 +2553,10 @@
         <v>100</v>
       </c>
       <c r="C56" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F56" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -2570,7 +2573,7 @@
         <v>101</v>
       </c>
       <c r="F57" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -2587,7 +2590,7 @@
         <v>101</v>
       </c>
       <c r="F58" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -2604,7 +2607,7 @@
         <v>105</v>
       </c>
       <c r="F59" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -2621,7 +2624,7 @@
         <v>101</v>
       </c>
       <c r="F60" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -2632,10 +2635,10 @@
         <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F61" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -2643,7 +2646,7 @@
         <v>107</v>
       </c>
       <c r="C62" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D62" t="s">
         <v>107</v>
@@ -2652,7 +2655,7 @@
         <v>108</v>
       </c>
       <c r="F62" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G62" t="s">
         <v>109</v>
@@ -2672,7 +2675,7 @@
         <v>111</v>
       </c>
       <c r="F63" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -2689,7 +2692,7 @@
         <v>111</v>
       </c>
       <c r="F64" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2706,7 +2709,7 @@
         <v>111</v>
       </c>
       <c r="F65" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -2714,7 +2717,7 @@
         <v>107</v>
       </c>
       <c r="C66" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D66" t="s">
         <v>114</v>
@@ -2723,7 +2726,7 @@
         <v>115</v>
       </c>
       <c r="F66" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2734,10 +2737,10 @@
         <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F67" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2830,7 +2833,7 @@
         <v>116</v>
       </c>
       <c r="C73" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="D73" t="s">
         <v>127</v>
@@ -2847,7 +2850,7 @@
         <v>116</v>
       </c>
       <c r="C74" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="D74" t="s">
         <v>129</v>
@@ -2856,7 +2859,7 @@
         <v>117</v>
       </c>
       <c r="F74" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2867,13 +2870,13 @@
         <v>117</v>
       </c>
       <c r="D75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E75" t="s">
         <v>117</v>
       </c>
       <c r="F75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2884,13 +2887,13 @@
         <v>117</v>
       </c>
       <c r="D76" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E76" t="s">
         <v>117</v>
       </c>
       <c r="F76" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2898,16 +2901,16 @@
         <v>116</v>
       </c>
       <c r="C77" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D77" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E77" t="s">
         <v>117</v>
       </c>
       <c r="F77" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2915,16 +2918,16 @@
         <v>116</v>
       </c>
       <c r="C78" t="s">
-        <v>138</v>
+        <v>243</v>
       </c>
       <c r="D78" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E78" t="s">
         <v>117</v>
       </c>
       <c r="F78" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2932,16 +2935,16 @@
         <v>116</v>
       </c>
       <c r="C79" t="s">
-        <v>140</v>
+        <v>244</v>
       </c>
       <c r="D79" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E79" t="s">
         <v>117</v>
       </c>
       <c r="F79" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -2949,16 +2952,16 @@
         <v>116</v>
       </c>
       <c r="C80" t="s">
-        <v>143</v>
+        <v>245</v>
       </c>
       <c r="D80" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E80" t="s">
         <v>117</v>
       </c>
       <c r="F80" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -2966,13 +2969,13 @@
         <v>116</v>
       </c>
       <c r="C81" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D81" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E81" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F81" t="s">
         <v>16</v>
@@ -2986,13 +2989,13 @@
         <v>117</v>
       </c>
       <c r="D82" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E82" t="s">
         <v>117</v>
       </c>
       <c r="F82" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -3003,13 +3006,13 @@
         <v>117</v>
       </c>
       <c r="D83" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E83" t="s">
         <v>117</v>
       </c>
       <c r="F83" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -3020,13 +3023,13 @@
         <v>117</v>
       </c>
       <c r="D84" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E84" t="s">
         <v>117</v>
       </c>
       <c r="F84" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -3037,13 +3040,13 @@
         <v>117</v>
       </c>
       <c r="D85" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E85" t="s">
         <v>117</v>
       </c>
       <c r="F85" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -3054,13 +3057,13 @@
         <v>117</v>
       </c>
       <c r="D86" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E86" t="s">
         <v>117</v>
       </c>
       <c r="F86" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -3068,16 +3071,16 @@
         <v>116</v>
       </c>
       <c r="C87" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D87" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E87" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F87" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -3085,16 +3088,16 @@
         <v>116</v>
       </c>
       <c r="C88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D88" t="s">
+        <v>155</v>
+      </c>
+      <c r="E88" t="s">
+        <v>153</v>
+      </c>
+      <c r="F88" t="s">
         <v>156</v>
-      </c>
-      <c r="D88" t="s">
-        <v>158</v>
-      </c>
-      <c r="E88" t="s">
-        <v>156</v>
-      </c>
-      <c r="F88" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -3102,13 +3105,13 @@
         <v>116</v>
       </c>
       <c r="C89" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D89" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E89" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F89" t="s">
         <v>16</v>
@@ -3119,13 +3122,13 @@
         <v>116</v>
       </c>
       <c r="C90" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D90" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E90" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F90" t="s">
         <v>16</v>
@@ -3136,7 +3139,7 @@
         <v>14</v>
       </c>
       <c r="B91" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C91" t="s">
         <v>88</v>
@@ -3150,47 +3153,47 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C92" t="s">
         <v>88</v>
       </c>
       <c r="D92" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E92" t="s">
         <v>88</v>
       </c>
       <c r="F92" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C93" t="s">
         <v>88</v>
       </c>
       <c r="D93" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E93" t="s">
         <v>88</v>
       </c>
       <c r="F93" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C94" t="s">
         <v>88</v>
       </c>
       <c r="D94" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E94" t="s">
         <v>88</v>
@@ -3199,7 +3202,7 @@
         <v>89</v>
       </c>
       <c r="G94" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -3207,67 +3210,67 @@
         <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C95" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F95" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C96" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D96" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E96" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F96" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
+        <v>166</v>
+      </c>
+      <c r="C97" t="s">
+        <v>170</v>
+      </c>
+      <c r="D97" t="s">
         <v>169</v>
       </c>
-      <c r="C97" t="s">
-        <v>173</v>
-      </c>
-      <c r="D97" t="s">
-        <v>172</v>
-      </c>
       <c r="E97" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F97" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C98" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D98" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E98" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F98" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G98" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -3275,53 +3278,53 @@
         <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C99" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E99" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G99" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
+        <v>175</v>
+      </c>
+      <c r="C100" t="s">
+        <v>176</v>
+      </c>
+      <c r="D100" t="s">
         <v>178</v>
       </c>
-      <c r="C100" t="s">
+      <c r="E100" t="s">
+        <v>176</v>
+      </c>
+      <c r="F100" t="s">
         <v>179</v>
-      </c>
-      <c r="D100" t="s">
-        <v>181</v>
-      </c>
-      <c r="E100" t="s">
-        <v>179</v>
-      </c>
-      <c r="F100" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C101" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D101" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E101" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F101" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -3329,33 +3332,33 @@
         <v>17</v>
       </c>
       <c r="B102" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C102" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E102" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F102" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
+        <v>182</v>
+      </c>
+      <c r="C103" t="s">
+        <v>183</v>
+      </c>
+      <c r="D103" t="s">
         <v>185</v>
       </c>
-      <c r="C103" t="s">
-        <v>186</v>
-      </c>
-      <c r="D103" t="s">
-        <v>188</v>
-      </c>
       <c r="E103" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F103" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -3363,10 +3366,10 @@
         <v>18</v>
       </c>
       <c r="B104" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C104" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F104" t="s">
         <v>16</v>
@@ -3374,16 +3377,16 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
+        <v>186</v>
+      </c>
+      <c r="C105" t="s">
         <v>189</v>
       </c>
-      <c r="C105" t="s">
-        <v>192</v>
-      </c>
       <c r="D105" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E105" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F105" t="s">
         <v>16</v>
@@ -3391,16 +3394,16 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
+        <v>186</v>
+      </c>
+      <c r="C106" t="s">
         <v>189</v>
       </c>
-      <c r="C106" t="s">
-        <v>192</v>
-      </c>
       <c r="D106" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E106" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F106" t="s">
         <v>16</v>
@@ -3408,16 +3411,16 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C107" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D107" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E107" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F107" t="s">
         <v>16</v>
@@ -3425,16 +3428,16 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C108" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D108" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E108" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F108" t="s">
         <v>16</v>
@@ -3442,16 +3445,16 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C109" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D109" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E109" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F109" t="s">
         <v>16</v>
@@ -3459,16 +3462,16 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C110" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D110" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E110" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F110" t="s">
         <v>16</v>
@@ -3476,16 +3479,16 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C111" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D111" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E111" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F111" t="s">
         <v>16</v>
@@ -3493,16 +3496,16 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C112" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D112" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E112" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F112" t="s">
         <v>16</v>
@@ -3510,16 +3513,16 @@
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C113" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D113" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E113" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F113" t="s">
         <v>16</v>
@@ -3527,16 +3530,16 @@
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C114" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D114" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E114" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F114" t="s">
         <v>16</v>
@@ -3544,16 +3547,16 @@
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C115" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D115" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E115" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F115" t="s">
         <v>16</v>
@@ -3561,16 +3564,16 @@
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C116" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D116" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E116" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F116" t="s">
         <v>16</v>

</xml_diff>